<commit_message>
Working with this method
</commit_message>
<xml_diff>
--- a/tests/Questionarie.xlsx
+++ b/tests/Questionarie.xlsx
@@ -130,7 +130,7 @@
     <t>Durante el verano no puedo salir sin regresar a casa quemado y deshidratado.</t>
   </si>
   <si>
-    <t>Me molesta requerir de aire acondicionado para poder enfriar la temperaturad durante invierno</t>
+    <t>Me molesta requerir de aire acondicionado para poder enfriar la temperatura durante verano</t>
   </si>
   <si>
     <t>Durante la primavera disfruto de la naturaleza y el cantar de las aves.</t>
@@ -33771,28 +33771,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A38:A43"/>
     <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A38:A43"/>
     <mergeCell ref="A50:A55"/>
     <mergeCell ref="A56:A61"/>
     <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B63:B67"/>
-    <mergeCell ref="B21:B25"/>
     <mergeCell ref="B27:B31"/>
     <mergeCell ref="B33:B37"/>
     <mergeCell ref="B39:B43"/>
     <mergeCell ref="B45:B49"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B21:B25"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>